<commit_message>
Add page breaks; repeating rows
</commit_message>
<xml_diff>
--- a/test/files/borders.xlsx
+++ b/test/files/borders.xlsx
@@ -54,8 +54,12 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFFFAA00"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
       <top style="thick">
         <color rgb="FFFF0000"/>
       </top>

</xml_diff>